<commit_message>
Data and estimation updates
</commit_message>
<xml_diff>
--- a/archived/actualGDP.xlsx
+++ b/archived/actualGDP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsun\Dropbox\forecasting_competition_estimation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\archived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5156959D-AD16-4BF1-9387-2810742B96EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81602F5E-15A3-4406-9D16-AEAA95E32746}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C9337A89-BB6C-447B-BAD2-29D97D5558DD}"/>
+    <workbookView xWindow="-7335" yWindow="3885" windowWidth="27900" windowHeight="14865" activeTab="1" xr2:uid="{C9337A89-BB6C-447B-BAD2-29D97D5558DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="288">
   <si>
     <t>DATE</t>
   </si>
@@ -893,6 +893,9 @@
   </si>
   <si>
     <t>ROUTPUT12Q3</t>
+  </si>
+  <si>
+    <t>2020Q2</t>
   </si>
 </sst>
 </file>
@@ -919,7 +922,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -947,6 +950,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1032,13 +1041,17 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6957,19 +6970,19 @@
       <c r="G243" s="4">
         <v>13204</v>
       </c>
-      <c r="Z243" s="23" t="s">
+      <c r="Z243" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="AA243" s="23"/>
-      <c r="AB243" s="23"/>
-      <c r="AC243" s="23"/>
-      <c r="AD243" s="23"/>
-      <c r="AF243" s="23" t="s">
+      <c r="AA243" s="25"/>
+      <c r="AB243" s="25"/>
+      <c r="AC243" s="25"/>
+      <c r="AD243" s="25"/>
+      <c r="AF243" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="AG243" s="23"/>
-      <c r="AH243" s="23"/>
-      <c r="AI243" s="23"/>
+      <c r="AG243" s="25"/>
+      <c r="AH243" s="25"/>
+      <c r="AI243" s="25"/>
     </row>
     <row r="244" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
@@ -8290,10 +8303,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF94E8A-04A7-4AE2-A246-DDF55432B9CA}">
-  <dimension ref="A1:AI291"/>
+  <dimension ref="A1:AJ291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F219" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD227" sqref="AD227"/>
+    <sheetView tabSelected="1" topLeftCell="L237" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q248" sqref="Q248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17421,7 +17434,7 @@
         <v>12950.4</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>244</v>
       </c>
@@ -17459,7 +17472,7 @@
         <v>13038.4</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>245</v>
       </c>
@@ -17497,7 +17510,7 @@
         <v>13056.1</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>246</v>
       </c>
@@ -17535,28 +17548,29 @@
         <v>13173.6</v>
       </c>
       <c r="N243" s="8"/>
-      <c r="O243" s="24" t="s">
+      <c r="O243" s="26" t="s">
         <v>283</v>
       </c>
-      <c r="P243" s="24"/>
-      <c r="Q243" s="24"/>
-      <c r="R243" s="24"/>
-      <c r="S243" s="24"/>
-      <c r="T243" s="24"/>
-      <c r="U243" s="24"/>
-      <c r="V243" s="24"/>
-      <c r="W243" s="24"/>
-      <c r="X243" s="24"/>
+      <c r="P243" s="26"/>
+      <c r="Q243" s="26"/>
+      <c r="R243" s="26"/>
+      <c r="S243" s="26"/>
+      <c r="T243" s="26"/>
+      <c r="U243" s="26"/>
+      <c r="V243" s="26"/>
+      <c r="W243" s="26"/>
+      <c r="X243" s="26"/>
       <c r="Y243" s="15"/>
-      <c r="Z243" s="8"/>
-      <c r="AA243" s="24" t="s">
+      <c r="Z243" s="23"/>
+      <c r="AA243" s="8"/>
+      <c r="AB243" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="AB243" s="24"/>
-      <c r="AC243" s="24"/>
-      <c r="AD243" s="24"/>
-    </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AC243" s="26"/>
+      <c r="AD243" s="26"/>
+      <c r="AE243" s="26"/>
+    </row>
+    <row r="244" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>247</v>
       </c>
@@ -17627,21 +17641,24 @@
       <c r="Y244" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="Z244" s="7"/>
-      <c r="AA244" s="7" t="s">
+      <c r="Z244" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="AA244" s="7"/>
+      <c r="AB244" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="AB244" s="7" t="s">
+      <c r="AC244" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="AC244" s="7" t="s">
+      <c r="AD244" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="AD244" s="7" t="s">
+      <c r="AE244" s="7" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>248</v>
       </c>
@@ -17725,10 +17742,8 @@
         <f t="shared" si="0"/>
         <v>1.690494999943823</v>
       </c>
-      <c r="Z245" s="10"/>
-      <c r="AA245" s="9">
-        <v>-0.17192170149000799</v>
-      </c>
+      <c r="Z245" s="16"/>
+      <c r="AA245" s="10"/>
       <c r="AB245" s="9">
         <v>-0.17192170149000799</v>
       </c>
@@ -17738,20 +17753,23 @@
       <c r="AD245" s="9">
         <v>-0.17192170149000799</v>
       </c>
-      <c r="AF245" s="25">
+      <c r="AE245" s="9">
+        <v>-0.17192170149000799</v>
+      </c>
+      <c r="AG245" s="24">
         <v>-0.17206965644932687</v>
       </c>
-      <c r="AG245" s="25">
+      <c r="AH245" s="24">
         <v>-0.17206965644932687</v>
       </c>
-      <c r="AH245" s="25">
+      <c r="AI245" s="24">
         <v>-0.17206965644932687</v>
       </c>
-      <c r="AI245" s="25">
+      <c r="AJ245" s="24">
         <v>-0.17206965644932687</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>249</v>
       </c>
@@ -17835,10 +17853,8 @@
         <f t="shared" si="1"/>
         <v>-1.7809361269240993</v>
       </c>
-      <c r="Z246" s="10"/>
-      <c r="AA246" s="9">
-        <v>0.87370787668128502</v>
-      </c>
+      <c r="Z246" s="16"/>
+      <c r="AA246" s="10"/>
       <c r="AB246" s="9">
         <v>0.87370787668128502</v>
       </c>
@@ -17848,20 +17864,23 @@
       <c r="AD246" s="9">
         <v>0.87370787668128502</v>
       </c>
-      <c r="AF246" s="25">
+      <c r="AE246" s="9">
+        <v>0.87370787668128502</v>
+      </c>
+      <c r="AG246" s="24">
         <v>0.86991313668859671</v>
       </c>
-      <c r="AG246" s="25">
+      <c r="AH246" s="24">
         <v>0.86991313668859671</v>
       </c>
-      <c r="AH246" s="25">
+      <c r="AI246" s="24">
         <v>0.86991313668859671</v>
       </c>
-      <c r="AI246" s="25">
+      <c r="AJ246" s="24">
         <v>0.86991313668859671</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>250</v>
       </c>
@@ -17945,12 +17964,10 @@
         <f t="shared" si="1"/>
         <v>1.3154094473821587</v>
       </c>
-      <c r="Z247" s="10"/>
-      <c r="AA247" s="9">
+      <c r="Z247" s="16"/>
+      <c r="AA247" s="10"/>
+      <c r="AB247" s="9">
         <v>1.88855138949148</v>
-      </c>
-      <c r="AB247" s="9">
-        <v>2.8252586136575002</v>
       </c>
       <c r="AC247" s="9">
         <v>2.8252586136575002</v>
@@ -17958,20 +17975,23 @@
       <c r="AD247" s="9">
         <v>2.8252586136575002</v>
       </c>
-      <c r="AF247" s="25">
+      <c r="AE247" s="9">
+        <v>2.8252586136575002</v>
+      </c>
+      <c r="AG247" s="24">
         <v>1.8709396500739373</v>
       </c>
-      <c r="AG247" s="25">
+      <c r="AH247" s="24">
         <v>2.7860843210645769</v>
       </c>
-      <c r="AH247" s="25">
+      <c r="AI247" s="24">
         <v>2.7860843210645769</v>
       </c>
-      <c r="AI247" s="25">
+      <c r="AJ247" s="24">
         <v>2.7860843210645769</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>251</v>
       </c>
@@ -18011,7 +18031,9 @@
       <c r="N248" t="s">
         <v>268</v>
       </c>
-      <c r="O248" s="10"/>
+      <c r="O248" s="27">
+        <v>2</v>
+      </c>
       <c r="P248" s="9">
         <f t="shared" si="1"/>
         <v>-0.25248002748920989</v>
@@ -18052,33 +18074,36 @@
         <f t="shared" si="1"/>
         <v>-3.7317139482342934</v>
       </c>
-      <c r="Z248" s="10"/>
-      <c r="AA248" s="11">
+      <c r="Z248" s="16">
+        <v>-0.7</v>
+      </c>
+      <c r="AA248" s="10"/>
+      <c r="AB248" s="11">
         <v>-0.51064160084837196</v>
       </c>
-      <c r="AB248" s="9">
+      <c r="AC248" s="9">
         <v>-0.25216156474245899</v>
-      </c>
-      <c r="AC248" s="9">
-        <v>-0.51064160084838295</v>
       </c>
       <c r="AD248" s="9">
         <v>-0.51064160084838295</v>
       </c>
-      <c r="AF248">
+      <c r="AE248" s="9">
+        <v>-0.51064160084838295</v>
+      </c>
+      <c r="AG248">
         <v>-0.51194983054801591</v>
       </c>
-      <c r="AG248" s="25">
+      <c r="AH248" s="24">
         <v>-0.25248002748920989</v>
       </c>
-      <c r="AH248" s="25">
+      <c r="AI248" s="24">
         <v>-0.51194983054801591</v>
       </c>
-      <c r="AI248" s="25">
+      <c r="AJ248" s="24">
         <v>-0.51194983054801591</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>252</v>
       </c>
@@ -18156,33 +18181,34 @@
         <f t="shared" si="2"/>
         <v>-9.3105958714611337</v>
       </c>
-      <c r="Z249" s="10"/>
-      <c r="AA249" s="11">
-        <v>-6.3424103134836303</v>
-      </c>
+      <c r="Z249" s="16"/>
+      <c r="AA249" s="10"/>
       <c r="AB249" s="11">
         <v>-6.3424103134836303</v>
       </c>
-      <c r="AC249" s="9">
+      <c r="AC249" s="11">
+        <v>-6.3424103134836303</v>
+      </c>
+      <c r="AD249" s="9">
         <v>-3.80366704542454</v>
       </c>
-      <c r="AD249" s="9">
+      <c r="AE249" s="9">
         <v>-6.3424103134836303</v>
-      </c>
-      <c r="AF249">
-        <v>-6.5524717279658526</v>
       </c>
       <c r="AG249">
         <v>-6.5524717279658526</v>
       </c>
-      <c r="AH249" s="25">
+      <c r="AH249">
+        <v>-6.5524717279658526</v>
+      </c>
+      <c r="AI249" s="24">
         <v>-3.8778948018284263</v>
       </c>
-      <c r="AI249" s="25">
+      <c r="AJ249" s="24">
         <v>-6.5524717279658526</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>253</v>
       </c>
@@ -18222,9 +18248,9 @@
       <c r="N250" t="s">
         <v>270</v>
       </c>
-      <c r="O250" s="10"/>
-      <c r="P250" s="10"/>
-      <c r="Q250" s="10"/>
+      <c r="O250" s="27"/>
+      <c r="P250" s="27"/>
+      <c r="Q250" s="27"/>
       <c r="R250" s="9">
         <f t="shared" ref="R250:Y250" si="3">LN(E250/E249)*100*4</f>
         <v>-6.3405080366300677</v>
@@ -18257,21 +18283,19 @@
         <f t="shared" si="3"/>
         <v>-5.3918650318880879</v>
       </c>
-      <c r="Z250" s="10"/>
-      <c r="AA250" s="11">
-        <v>-6.4285552263160204</v>
-      </c>
+      <c r="Z250" s="16"/>
+      <c r="AA250" s="10"/>
       <c r="AB250" s="11">
         <v>-6.4285552263160204</v>
       </c>
       <c r="AC250" s="11">
         <v>-6.4285552263160204</v>
       </c>
-      <c r="AD250" s="9">
+      <c r="AD250" s="11">
+        <v>-6.4285552263160204</v>
+      </c>
+      <c r="AE250" s="9">
         <v>-6.1436796851859397</v>
-      </c>
-      <c r="AF250">
-        <v>-6.6444926254293284</v>
       </c>
       <c r="AG250">
         <v>-6.6444926254293284</v>
@@ -18279,11 +18303,14 @@
       <c r="AH250">
         <v>-6.6444926254293284</v>
       </c>
-      <c r="AI250" s="25">
+      <c r="AI250">
+        <v>-6.6444926254293284</v>
+      </c>
+      <c r="AJ250" s="24">
         <v>-6.3405080366300677</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>254</v>
       </c>
@@ -18355,10 +18382,8 @@
         <f t="shared" si="4"/>
         <v>-0.31481191613977122</v>
       </c>
-      <c r="Z251" s="10"/>
-      <c r="AA251" s="11">
-        <v>-0.70259705541280104</v>
-      </c>
+      <c r="Z251" s="17"/>
+      <c r="AA251" s="10"/>
       <c r="AB251" s="11">
         <v>-0.70259705541280104</v>
       </c>
@@ -18368,8 +18393,8 @@
       <c r="AD251" s="11">
         <v>-0.70259705541280104</v>
       </c>
-      <c r="AF251">
-        <v>-0.74031360549679592</v>
+      <c r="AE251" s="11">
+        <v>-0.70259705541280104</v>
       </c>
       <c r="AG251">
         <v>-0.74031360549679592</v>
@@ -18380,8 +18405,11 @@
       <c r="AI251">
         <v>-0.74031360549679592</v>
       </c>
-    </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ251">
+        <v>-0.74031360549679592</v>
+      </c>
+    </row>
+    <row r="252" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>255</v>
       </c>
@@ -18450,10 +18478,8 @@
         <f t="shared" si="5"/>
         <v>1.4366736209002471</v>
       </c>
-      <c r="Z252" s="10"/>
-      <c r="AA252" s="11">
-        <v>1.5957215413791199</v>
-      </c>
+      <c r="Z252" s="17"/>
+      <c r="AA252" s="10"/>
       <c r="AB252" s="11">
         <v>1.5957215413791199</v>
       </c>
@@ -18463,8 +18489,8 @@
       <c r="AD252" s="11">
         <v>1.5957215413791199</v>
       </c>
-      <c r="AF252">
-        <v>2.2106763645474294</v>
+      <c r="AE252" s="11">
+        <v>1.5957215413791199</v>
       </c>
       <c r="AG252">
         <v>2.2106763645474294</v>
@@ -18475,8 +18501,11 @@
       <c r="AI252">
         <v>2.2106763645474294</v>
       </c>
-    </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ252">
+        <v>2.2106763645474294</v>
+      </c>
+    </row>
+    <row r="253" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>256</v>
       </c>
@@ -18542,11 +18571,9 @@
         <f>LN(L253/L252)*100*4</f>
         <v>3.9469793079573523</v>
       </c>
-      <c r="Z253" s="10"/>
-      <c r="AA253" s="10">
-        <v>5.0119129678187297</v>
-      </c>
-      <c r="AB253" s="11">
+      <c r="Z253" s="17"/>
+      <c r="AA253" s="10"/>
+      <c r="AB253" s="10">
         <v>5.0119129678187297</v>
       </c>
       <c r="AC253" s="11">
@@ -18555,8 +18582,8 @@
       <c r="AD253" s="11">
         <v>5.0119129678187297</v>
       </c>
-      <c r="AF253">
-        <v>5.4053841993297649</v>
+      <c r="AE253" s="11">
+        <v>5.0119129678187297</v>
       </c>
       <c r="AG253">
         <v>5.4053841993297649</v>
@@ -18567,8 +18594,11 @@
       <c r="AI253">
         <v>5.4053841993297649</v>
       </c>
-    </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ253">
+        <v>5.4053841993297649</v>
+      </c>
+    </row>
+    <row r="254" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>257</v>
       </c>
@@ -18608,13 +18638,13 @@
       <c r="N254" t="s">
         <v>265</v>
       </c>
-      <c r="O254" s="10"/>
-      <c r="P254" s="10"/>
-      <c r="Q254" s="10"/>
-      <c r="R254" s="10"/>
-      <c r="S254" s="10"/>
-      <c r="T254" s="10"/>
-      <c r="U254" s="10"/>
+      <c r="O254" s="27"/>
+      <c r="P254" s="27"/>
+      <c r="Q254" s="27"/>
+      <c r="R254" s="27"/>
+      <c r="S254" s="27"/>
+      <c r="T254" s="27"/>
+      <c r="U254" s="27"/>
       <c r="V254" s="10">
         <f>LN(I254/I253)*100*4</f>
         <v>3.1873885715874302</v>
@@ -18631,21 +18661,19 @@
         <f>LN(L254/L253)*100*4</f>
         <v>2.3082319762007568</v>
       </c>
-      <c r="Z254" s="10"/>
-      <c r="AA254" s="10">
-        <v>3.7318920134817399</v>
-      </c>
+      <c r="Z254" s="17"/>
+      <c r="AA254" s="10"/>
       <c r="AB254" s="10">
         <v>3.7318920134817399</v>
       </c>
-      <c r="AC254" s="11">
+      <c r="AC254" s="10">
         <v>3.7318920134817399</v>
       </c>
       <c r="AD254" s="11">
         <v>3.7318920134817399</v>
       </c>
-      <c r="AF254">
-        <v>3.6639423079929583</v>
+      <c r="AE254" s="11">
+        <v>3.7318920134817399</v>
       </c>
       <c r="AG254">
         <v>3.6639423079929583</v>
@@ -18656,8 +18684,11 @@
       <c r="AI254">
         <v>3.6639423079929583</v>
       </c>
-    </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ254">
+        <v>3.6639423079929583</v>
+      </c>
+    </row>
+    <row r="255" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>259</v>
       </c>
@@ -18717,21 +18748,19 @@
         <f>LN(L255/L254)*100*4</f>
         <v>2.2181886229839285</v>
       </c>
-      <c r="Z255" s="12"/>
-      <c r="AA255" s="12">
-        <v>1.71888839835925</v>
-      </c>
+      <c r="Z255" s="18"/>
+      <c r="AA255" s="12"/>
       <c r="AB255" s="12">
         <v>1.71888839835925</v>
       </c>
       <c r="AC255" s="12">
         <v>1.71888839835925</v>
       </c>
-      <c r="AD255" s="13">
+      <c r="AD255" s="12">
         <v>1.71888839835925</v>
       </c>
-      <c r="AF255">
-        <v>1.7042826452235225</v>
+      <c r="AE255" s="13">
+        <v>1.71888839835925</v>
       </c>
       <c r="AG255">
         <v>1.7042826452235225</v>
@@ -18742,8 +18771,11 @@
       <c r="AI255">
         <v>1.7042826452235225</v>
       </c>
-    </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ255">
+        <v>1.7042826452235225</v>
+      </c>
+    </row>
+    <row r="256" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>260</v>
       </c>
@@ -18800,10 +18832,8 @@
         <f>LN(L256/L255)*100*4</f>
         <v>2.5693823009197909</v>
       </c>
-      <c r="Z256" s="14"/>
-      <c r="AA256" s="14">
-        <v>2.0096804996220201</v>
-      </c>
+      <c r="Z256" s="22"/>
+      <c r="AA256" s="14"/>
       <c r="AB256" s="14">
         <v>2.0096804996220201</v>
       </c>
@@ -18813,8 +18843,8 @@
       <c r="AD256" s="14">
         <v>2.0096804996220201</v>
       </c>
-      <c r="AF256">
-        <v>2.5693823009197909</v>
+      <c r="AE256" s="14">
+        <v>2.0096804996220201</v>
       </c>
       <c r="AG256">
         <v>2.5693823009197909</v>
@@ -18823,6 +18853,9 @@
         <v>2.5693823009197909</v>
       </c>
       <c r="AI256">
+        <v>2.5693823009197909</v>
+      </c>
+      <c r="AJ256">
         <v>2.5693823009197909</v>
       </c>
     </row>
@@ -19034,7 +19067,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="O243:X243"/>
-    <mergeCell ref="AA243:AD243"/>
+    <mergeCell ref="AB243:AE243"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>